<commit_message>
Nott supp files and plot
</commit_message>
<xml_diff>
--- a/echolocatoR/annotations/Glass_lab/Glass.snEpigenomics.xlsx
+++ b/echolocatoR/annotations/Glass_lab/Glass.snEpigenomics.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schilder/Desktop/Fine_Mapping/echolocatoR/tools/Annotations/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schilder/Desktop/Fine_Mapping/echolocatoR/annotations/Glass_lab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{827CE40D-2EC1-F44B-B192-80DC59ED2A6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ECA2358-FCF3-4140-A4AD-A27930EB2587}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="1740" windowWidth="18540" windowHeight="18080" xr2:uid="{010F0F86-E4AD-7D4F-87C8-55A1C5C6F5BF}"/>
+    <workbookView xWindow="900" yWindow="460" windowWidth="18540" windowHeight="17540" xr2:uid="{010F0F86-E4AD-7D4F-87C8-55A1C5C6F5BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="67">
   <si>
     <t> schema </t>
   </si>
@@ -214,13 +214,34 @@
   </si>
   <si>
     <t>assay_path</t>
+  </si>
+  <si>
+    <t>open chromatin</t>
+  </si>
+  <si>
+    <t>active promoters</t>
+  </si>
+  <si>
+    <t>﻿active promoters &amp; enhancers</t>
+  </si>
+  <si>
+    <t>functional_association</t>
+  </si>
+  <si>
+    <t>fresh_frozen</t>
+  </si>
+  <si>
+    <t>fresh</t>
+  </si>
+  <si>
+    <t>frozen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -250,6 +271,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -272,12 +300,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -593,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F20365B-2B7B-E647-B034-C96F4CC885A9}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -604,13 +633,14 @@
     <col min="1" max="1" width="34.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="52.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="17.83203125" customWidth="1"/>
-    <col min="9" max="9" width="108.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.83203125" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="17.83203125" customWidth="1"/>
+    <col min="11" max="11" width="108.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -624,22 +654,28 @@
         <v>4</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
@@ -653,24 +689,30 @@
         <v>5</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="2" t="str">
+      <c r="I2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="2" t="str">
         <f>"nuclei_"&amp;LOWER(D2)&amp;"_hg19_pooled/hg19"</f>
         <v>nuclei_h3k27ac_hg19_pooled/hg19</v>
       </c>
-      <c r="I2" s="2" t="str">
-        <f>G2&amp;H2&amp;"/"&amp;B2&amp;".ucsc.bigWig"</f>
+      <c r="K2" s="2" t="str">
+        <f>I2&amp;J2&amp;"/"&amp;B2&amp;".ucsc.bigWig"</f>
         <v>http://homer.ucsd.edu/hubs//nuclei_h3k27ac_hg19_pooled/hg19/human_microglia_H3K27ac_exvivo_pooled_hg19.ucsc.bigWig</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -684,24 +726,30 @@
         <v>5</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="2" t="str">
-        <f t="shared" ref="H3:H19" si="0">"nuclei_"&amp;LOWER(D3)&amp;"_hg19_pooled/hg19"</f>
+      <c r="I3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="2" t="str">
+        <f t="shared" ref="J3:J19" si="0">"nuclei_"&amp;LOWER(D3)&amp;"_hg19_pooled/hg19"</f>
         <v>nuclei_h3k27ac_hg19_pooled/hg19</v>
       </c>
-      <c r="I3" s="2" t="str">
-        <f t="shared" ref="I3:I19" si="1">G3&amp;H3&amp;"/"&amp;B3&amp;".ucsc.bigWig"</f>
+      <c r="K3" s="2" t="str">
+        <f t="shared" ref="K3:K19" si="1">I3&amp;J3&amp;"/"&amp;B3&amp;".ucsc.bigWig"</f>
         <v>http://homer.ucsd.edu/hubs//nuclei_h3k27ac_hg19_pooled/hg19/human_microglia_H3K27ac_exvivo_pooled_hg19_tbp.ucsc.bigWig</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
@@ -715,24 +763,30 @@
         <v>5</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="2" t="str">
+      <c r="I4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>nuclei_h3k27ac_hg19_pooled/hg19</v>
       </c>
-      <c r="I4" s="2" t="str">
+      <c r="K4" s="2" t="str">
         <f t="shared" si="1"/>
         <v>http://homer.ucsd.edu/hubs//nuclei_h3k27ac_hg19_pooled/hg19/human_PU1nuclei_H3K27ac_epilepsy_pooled_hg19.ucsc.bigWig</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>29</v>
       </c>
@@ -746,24 +800,30 @@
         <v>5</v>
       </c>
       <c r="E5" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="2" t="str">
+      <c r="I5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="2" t="str">
         <f t="shared" si="0"/>
         <v>nuclei_h3k27ac_hg19_pooled/hg19</v>
       </c>
-      <c r="I5" s="2" t="str">
+      <c r="K5" s="2" t="str">
         <f t="shared" si="1"/>
         <v>http://homer.ucsd.edu/hubs//nuclei_h3k27ac_hg19_pooled/hg19/human_NEUNnuclei_H3K27ac_epilepsy_pooled_hg19.ucsc.bigWig</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
@@ -777,24 +837,30 @@
         <v>5</v>
       </c>
       <c r="E6" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="2" t="str">
+      <c r="I6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="2" t="str">
         <f t="shared" si="0"/>
         <v>nuclei_h3k27ac_hg19_pooled/hg19</v>
       </c>
-      <c r="I6" s="2" t="str">
+      <c r="K6" s="2" t="str">
         <f t="shared" si="1"/>
         <v>http://homer.ucsd.edu/hubs//nuclei_h3k27ac_hg19_pooled/hg19/human_OLIG2nuclei_H3K27ac_epilepsy_pooled_hg19.ucsc.bigWig</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>33</v>
       </c>
@@ -808,24 +874,30 @@
         <v>5</v>
       </c>
       <c r="E7" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="2" t="str">
+      <c r="I7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>nuclei_h3k27ac_hg19_pooled/hg19</v>
       </c>
-      <c r="I7" s="2" t="str">
+      <c r="K7" s="2" t="str">
         <f t="shared" si="1"/>
         <v>http://homer.ucsd.edu/hubs//nuclei_h3k27ac_hg19_pooled/hg19/human_peripheralPU1nuclei_H3K27ac_hg19.ucsc.bigWig</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>35</v>
       </c>
@@ -839,24 +911,30 @@
         <v>5</v>
       </c>
       <c r="E8" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" s="2" t="str">
+      <c r="I8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>nuclei_h3k27ac_hg19_pooled/hg19</v>
       </c>
-      <c r="I8" s="2" t="str">
+      <c r="K8" s="2" t="str">
         <f t="shared" si="1"/>
         <v>http://homer.ucsd.edu/hubs//nuclei_h3k27ac_hg19_pooled/hg19/human_LHX2nuclei_H3K27ac_epilepsy_pooled_hg19.ucsc.bigWig</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
@@ -870,24 +948,30 @@
         <v>6</v>
       </c>
       <c r="E9" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="H9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="2" t="str">
+      <c r="I9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" s="2" t="str">
         <f t="shared" si="0"/>
         <v>nuclei_atac_hg19_pooled/hg19</v>
       </c>
-      <c r="I9" s="2" t="str">
+      <c r="K9" s="2" t="str">
         <f t="shared" si="1"/>
         <v>http://homer.ucsd.edu/hubs//nuclei_atac_hg19_pooled/hg19/human_microglia_atac_exvivo_pooled_hg19.ucsc.bigWig</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>39</v>
       </c>
@@ -901,24 +985,30 @@
         <v>6</v>
       </c>
       <c r="E10" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="H10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H10" s="2" t="str">
+      <c r="I10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>nuclei_atac_hg19_pooled/hg19</v>
       </c>
-      <c r="I10" s="2" t="str">
+      <c r="K10" s="2" t="str">
         <f t="shared" si="1"/>
         <v>http://homer.ucsd.edu/hubs//nuclei_atac_hg19_pooled/hg19/human_microglia_atac_exvivo_pooled_hg19_tbp.ucsc.bigWig</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>41</v>
       </c>
@@ -932,24 +1022,30 @@
         <v>6</v>
       </c>
       <c r="E11" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="H11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H11" s="2" t="str">
+      <c r="I11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J11" s="2" t="str">
         <f t="shared" si="0"/>
         <v>nuclei_atac_hg19_pooled/hg19</v>
       </c>
-      <c r="I11" s="2" t="str">
+      <c r="K11" s="2" t="str">
         <f t="shared" si="1"/>
         <v>http://homer.ucsd.edu/hubs//nuclei_atac_hg19_pooled/hg19/human_PU1nuclei_atac_epilepsy_pooled_hg19.ucsc.bigWig</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>43</v>
       </c>
@@ -963,24 +1059,30 @@
         <v>6</v>
       </c>
       <c r="E12" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="H12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H12" s="2" t="str">
+      <c r="I12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" s="2" t="str">
         <f t="shared" si="0"/>
         <v>nuclei_atac_hg19_pooled/hg19</v>
       </c>
-      <c r="I12" s="2" t="str">
+      <c r="K12" s="2" t="str">
         <f t="shared" si="1"/>
         <v>http://homer.ucsd.edu/hubs//nuclei_atac_hg19_pooled/hg19/human_NEUNnuclei_atac_epilepsy_pooled_hg19.ucsc.bigWig</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>45</v>
       </c>
@@ -994,24 +1096,30 @@
         <v>6</v>
       </c>
       <c r="E13" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="H13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H13" s="2" t="str">
+      <c r="I13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" s="2" t="str">
         <f t="shared" si="0"/>
         <v>nuclei_atac_hg19_pooled/hg19</v>
       </c>
-      <c r="I13" s="2" t="str">
+      <c r="K13" s="2" t="str">
         <f t="shared" si="1"/>
         <v>http://homer.ucsd.edu/hubs//nuclei_atac_hg19_pooled/hg19/human_OLIG2nuclei_atac_epilepsy_pooled_hg19.ucsc.bigWig</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>47</v>
       </c>
@@ -1025,24 +1133,30 @@
         <v>6</v>
       </c>
       <c r="E14" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="H14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H14" s="2" t="str">
+      <c r="I14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" s="2" t="str">
         <f t="shared" si="0"/>
         <v>nuclei_atac_hg19_pooled/hg19</v>
       </c>
-      <c r="I14" s="2" t="str">
+      <c r="K14" s="2" t="str">
         <f t="shared" si="1"/>
         <v>http://homer.ucsd.edu/hubs//nuclei_atac_hg19_pooled/hg19/human_peripheralPU1nuclei_atac_hg19.ucsc.bigWig</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>49</v>
       </c>
@@ -1056,24 +1170,30 @@
         <v>6</v>
       </c>
       <c r="E15" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="H15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H15" s="2" t="str">
+      <c r="I15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15" s="2" t="str">
         <f t="shared" si="0"/>
         <v>nuclei_atac_hg19_pooled/hg19</v>
       </c>
-      <c r="I15" s="2" t="str">
+      <c r="K15" s="2" t="str">
         <f t="shared" si="1"/>
         <v>http://homer.ucsd.edu/hubs//nuclei_atac_hg19_pooled/hg19/human_LHX2nuclei_atac_epilepsy_pooled_hg19.ucsc.bigWig</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>51</v>
       </c>
@@ -1086,25 +1206,31 @@
       <c r="D16" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="H16" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H16" s="2" t="str">
+      <c r="I16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" s="2" t="str">
         <f t="shared" si="0"/>
         <v>nuclei_h3k4me3_hg19_pooled/hg19</v>
       </c>
-      <c r="I16" s="2" t="str">
+      <c r="K16" s="2" t="str">
         <f t="shared" si="1"/>
         <v>http://homer.ucsd.edu/hubs//nuclei_h3k4me3_hg19_pooled/hg19/human_PU1nuclei_H3K4me3_epilepsy_hg19.ucsc.bigWig</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>53</v>
       </c>
@@ -1117,25 +1243,31 @@
       <c r="D17" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G17" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="H17" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H17" s="2" t="str">
+      <c r="I17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J17" s="2" t="str">
         <f t="shared" si="0"/>
         <v>nuclei_h3k4me3_hg19_pooled/hg19</v>
       </c>
-      <c r="I17" s="2" t="str">
+      <c r="K17" s="2" t="str">
         <f t="shared" si="1"/>
         <v>http://homer.ucsd.edu/hubs//nuclei_h3k4me3_hg19_pooled/hg19/human_NEUNnuclei_H3K4me3_epilepsy_hg19.ucsc.bigWig</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>55</v>
       </c>
@@ -1148,25 +1280,31 @@
       <c r="D18" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="H18" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H18" s="2" t="str">
+      <c r="I18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J18" s="2" t="str">
         <f t="shared" si="0"/>
         <v>nuclei_h3k4me3_hg19_pooled/hg19</v>
       </c>
-      <c r="I18" s="2" t="str">
+      <c r="K18" s="2" t="str">
         <f t="shared" si="1"/>
         <v>http://homer.ucsd.edu/hubs//nuclei_h3k4me3_hg19_pooled/hg19/human_OLIG2nuclei_H3K4me3_epilepsy_hg19.ucsc.bigWig</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>57</v>
       </c>
@@ -1179,25 +1317,31 @@
       <c r="D19" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="H19" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H19" s="2" t="str">
+      <c r="I19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J19" s="2" t="str">
         <f t="shared" si="0"/>
         <v>nuclei_h3k4me3_hg19_pooled/hg19</v>
       </c>
-      <c r="I19" s="2" t="str">
+      <c r="K19" s="2" t="str">
         <f t="shared" si="1"/>
         <v>http://homer.ucsd.edu/hubs//nuclei_h3k4me3_hg19_pooled/hg19/human_LHX2nuclei_H3K4me3_epilepsy_pooled_hg19.ucsc.bigWig</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
     </row>

</xml_diff>

<commit_message>
Add Nott histograms for all loci
</commit_message>
<xml_diff>
--- a/echolocatoR/annotations/Glass_lab/Glass.snEpigenomics.xlsx
+++ b/echolocatoR/annotations/Glass_lab/Glass.snEpigenomics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schilder/Desktop/Fine_Mapping/echolocatoR/annotations/Glass_lab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ECA2358-FCF3-4140-A4AD-A27930EB2587}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3858AA7A-4246-7C49-9DF7-0629E59BD481}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="460" windowWidth="18540" windowHeight="17540" xr2:uid="{010F0F86-E4AD-7D4F-87C8-55A1C5C6F5BF}"/>
+    <workbookView xWindow="900" yWindow="460" windowWidth="28500" windowHeight="17540" xr2:uid="{010F0F86-E4AD-7D4F-87C8-55A1C5C6F5BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -87,9 +87,6 @@
     <t>oligodendrocytes</t>
   </si>
   <si>
-    <t>neg</t>
-  </si>
-  <si>
     <t>peripheral microglia</t>
   </si>
   <si>
@@ -235,6 +232,9 @@
   </si>
   <si>
     <t>frozen</t>
+  </si>
+  <si>
+    <t>astrocytes</t>
   </si>
 </sst>
 </file>
@@ -625,7 +625,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -654,10 +654,10 @@
         <v>4</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>10</v>
@@ -666,21 +666,21 @@
         <v>8</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
@@ -689,10 +689,10 @@
         <v>5</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>11</v>
@@ -701,7 +701,7 @@
         <v>9</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J2" s="2" t="str">
         <f>"nuclei_"&amp;LOWER(D2)&amp;"_hg19_pooled/hg19"</f>
@@ -714,10 +714,10 @@
     </row>
     <row r="3" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>0</v>
@@ -726,10 +726,10 @@
         <v>5</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>11</v>
@@ -738,7 +738,7 @@
         <v>9</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J3" s="2" t="str">
         <f t="shared" ref="J3:J19" si="0">"nuclei_"&amp;LOWER(D3)&amp;"_hg19_pooled/hg19"</f>
@@ -751,10 +751,10 @@
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>0</v>
@@ -763,10 +763,10 @@
         <v>5</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>12</v>
@@ -775,7 +775,7 @@
         <v>9</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J4" s="2" t="str">
         <f t="shared" si="0"/>
@@ -788,10 +788,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>0</v>
@@ -800,10 +800,10 @@
         <v>5</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>13</v>
@@ -812,7 +812,7 @@
         <v>15</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J5" s="2" t="str">
         <f t="shared" si="0"/>
@@ -825,10 +825,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>0</v>
@@ -837,10 +837,10 @@
         <v>5</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>14</v>
@@ -849,7 +849,7 @@
         <v>16</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J6" s="2" t="str">
         <f t="shared" si="0"/>
@@ -862,10 +862,10 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>0</v>
@@ -874,19 +874,19 @@
         <v>5</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>12</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J7" s="2" t="str">
         <f t="shared" si="0"/>
@@ -899,10 +899,10 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>0</v>
@@ -911,19 +911,19 @@
         <v>5</v>
       </c>
       <c r="E8" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="I8" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J8" s="2" t="str">
         <f t="shared" si="0"/>
@@ -936,10 +936,10 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>0</v>
@@ -948,10 +948,10 @@
         <v>6</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>11</v>
@@ -960,7 +960,7 @@
         <v>9</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J9" s="2" t="str">
         <f t="shared" si="0"/>
@@ -973,10 +973,10 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>0</v>
@@ -985,10 +985,10 @@
         <v>6</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>11</v>
@@ -997,7 +997,7 @@
         <v>9</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J10" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1010,10 +1010,10 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>0</v>
@@ -1022,10 +1022,10 @@
         <v>6</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>12</v>
@@ -1034,7 +1034,7 @@
         <v>9</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J11" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1047,10 +1047,10 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>0</v>
@@ -1059,10 +1059,10 @@
         <v>6</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>13</v>
@@ -1071,7 +1071,7 @@
         <v>15</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J12" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1084,10 +1084,10 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>0</v>
@@ -1096,10 +1096,10 @@
         <v>6</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>14</v>
@@ -1108,7 +1108,7 @@
         <v>16</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J13" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1121,10 +1121,10 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>0</v>
@@ -1133,19 +1133,19 @@
         <v>6</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>12</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J14" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1158,10 +1158,10 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>0</v>
@@ -1170,19 +1170,19 @@
         <v>6</v>
       </c>
       <c r="E15" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="I15" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J15" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1195,10 +1195,10 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>0</v>
@@ -1207,10 +1207,10 @@
         <v>7</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>12</v>
@@ -1219,7 +1219,7 @@
         <v>9</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J16" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1232,10 +1232,10 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>0</v>
@@ -1244,10 +1244,10 @@
         <v>7</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>13</v>
@@ -1256,7 +1256,7 @@
         <v>15</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J17" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1269,10 +1269,10 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>0</v>
@@ -1281,10 +1281,10 @@
         <v>7</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>14</v>
@@ -1293,7 +1293,7 @@
         <v>16</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J18" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1306,10 +1306,10 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>0</v>
@@ -1318,19 +1318,19 @@
         <v>7</v>
       </c>
       <c r="E19" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F19" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="I19" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J19" s="2" t="str">
         <f t="shared" si="0"/>

</xml_diff>